<commit_message>
Implement GET and TRAFFIC jobs
</commit_message>
<xml_diff>
--- a/docs/orders-performance.xlsx
+++ b/docs/orders-performance.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\workspaces\bench_2017\spring-cloud-playground\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\workspaces\personal\orders-services\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="51">
   <si>
     <t xml:space="preserve">Job </t>
   </si>
@@ -175,6 +175,9 @@
   <si>
     <t>Increased memory up to 10G!!</t>
   </si>
+  <si>
+    <t>Client-Server latency</t>
+  </si>
 </sst>
 </file>
 
@@ -318,7 +321,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1219,7 +1221,7 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -1258,7 +1260,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
@@ -1321,7 +1323,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2769,12 +2770,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
+        <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
           <a:ln>
-            <a:noFill/>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -2885,6 +2888,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -3990,12 +3994,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
+        <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
           <a:ln>
-            <a:noFill/>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -4106,6 +4112,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -4579,8 +4586,428 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$116</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$D$100:$J$100</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0th</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50th</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v> 99th</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v> 99,9th</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v> 99,99th</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v> 99,999th</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v> 100th</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$116:$J$116</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.20100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.34499999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.3490000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.6649999999999991</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22.420999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>138.62700000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>141.74700000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-D154-472D-9882-2B43043B753E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$117</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent5">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent5">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$D$100:$J$100</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0th</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50th</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v> 99th</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v> 99,9th</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v> 99,99th</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v> 99,999th</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v> 100th</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$117:$J$117</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.187</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.46700000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.317</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.760000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>28.940999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>31.265000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-D154-472D-9882-2B43043B753E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$118</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent6">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent6">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$D$100:$J$100</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0th</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50th</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v> 99th</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v> 99,9th</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v> 99,99th</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v> 99,999th</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v> 100th</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$118:$J$118</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.186</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.778</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14.848000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26.225000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42.247999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>50.94</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-D154-472D-9882-2B43043B753E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>Sheet1!$C$116</c:f>
@@ -4714,13 +5141,13 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-ECE5-4387-84FC-5EC3DF81719F}"/>
+              <c16:uniqueId val="{00000001-D154-472D-9882-2B43043B753E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="4"/>
           <c:tx>
             <c:strRef>
               <c:f>Sheet1!$C$117</c:f>
@@ -4854,13 +5281,13 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-ECE5-4387-84FC-5EC3DF81719F}"/>
+              <c16:uniqueId val="{00000003-D154-472D-9882-2B43043B753E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="5"/>
           <c:tx>
             <c:strRef>
               <c:f>Sheet1!$C$118</c:f>
@@ -4994,7 +5421,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-ECE5-4387-84FC-5EC3DF81719F}"/>
+              <c16:uniqueId val="{00000005-D154-472D-9882-2B43043B753E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5208,12 +5635,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
+        <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
           <a:ln>
-            <a:noFill/>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -5324,6 +5753,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -7791,7 +8221,7 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -7830,7 +8260,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
@@ -7893,7 +8323,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9726,7 +10155,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11913,12 +12341,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
+        <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
           <a:ln>
-            <a:noFill/>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -12029,6 +12459,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -21937,15 +22368,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>217715</xdr:colOff>
+      <xdr:colOff>190501</xdr:colOff>
       <xdr:row>124</xdr:row>
-      <xdr:rowOff>70136</xdr:rowOff>
+      <xdr:rowOff>76940</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>122004</xdr:colOff>
+      <xdr:colOff>94790</xdr:colOff>
       <xdr:row>146</xdr:row>
-      <xdr:rowOff>124809</xdr:rowOff>
+      <xdr:rowOff>131613</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -22257,6 +22688,406 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.74923</cdr:x>
+      <cdr:y>0.92413</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.89259</cdr:x>
+      <cdr:y>0.96099</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="TextBox 2"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="2986767" y="3923560"/>
+          <a:ext cx="571500" cy="156482"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="pl-PL" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.76209</cdr:x>
+      <cdr:y>0.91924</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.95574</cdr:x>
+      <cdr:y>0.98503</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="4" name="TextBox 3"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="3038013" y="3902773"/>
+          <a:ext cx="771985" cy="279323"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="pl-PL" sz="900">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t># of threads</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.81312</cdr:x>
+      <cdr:y>0.92698</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.99364</cdr:x>
+      <cdr:y>0.98448</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="4" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="3268134" y="3935639"/>
+          <a:ext cx="725562" cy="244125"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="pl-PL" sz="900">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t># of threads</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.79611</cdr:x>
+      <cdr:y>0.91736</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.98976</cdr:x>
+      <cdr:y>0.98315</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="3173639" y="3894817"/>
+          <a:ext cx="771985" cy="279323"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="pl-PL" sz="900">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t># of threads</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.80707</cdr:x>
+      <cdr:y>0.88531</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>1</cdr:x>
+      <cdr:y>0.9511</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="3229414" y="3758746"/>
+          <a:ext cx="771985" cy="279323"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="pl-PL" sz="900">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t># of threads</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -22522,8 +23353,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A167" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="N148" sqref="N148"/>
+    <sheetView tabSelected="1" topLeftCell="A149" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="M182" sqref="M182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24597,7 +25428,7 @@
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="B97" s="4" t="s">
         <v>43</v>

</xml_diff>